<commit_message>
removed additional pod files and added a new test case
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Scenario (1)" sheetId="1" r:id="rId1"/>
+    <sheet name="Scenario (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Ticker</t>
   </si>
@@ -67,6 +69,18 @@
   </si>
   <si>
     <t>subtract new subtotal with actual subtotal and determine # of shares to buy + or sell -</t>
+  </si>
+  <si>
+    <t>RY</t>
+  </si>
+  <si>
+    <t>BMO</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>TD</t>
   </si>
 </sst>
 </file>
@@ -76,7 +90,7 @@
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -131,8 +145,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -148,11 +170,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -484,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -676,4 +706,250 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="B1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="100">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="19">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="C2" s="4">
+        <f>H2/SUM(H:H)</f>
+        <v>0.1395821242019733</v>
+      </c>
+      <c r="D2" s="2">
+        <f>C2</f>
+        <v>0.1395821242019733</v>
+      </c>
+      <c r="E2" s="2">
+        <f>B2-D2</f>
+        <v>0.26041787579802672</v>
+      </c>
+      <c r="F2" s="1">
+        <v>130</v>
+      </c>
+      <c r="G2" s="6">
+        <v>74</v>
+      </c>
+      <c r="H2" s="6">
+        <f>F2*G2</f>
+        <v>9620</v>
+      </c>
+      <c r="I2" s="8">
+        <f>B2*SUM(H:H)</f>
+        <v>27568</v>
+      </c>
+      <c r="J2" s="9">
+        <f>(I2-H2)/G2</f>
+        <v>242.54054054054055</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="19">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C5" si="0">H3/SUM(H:H)</f>
+        <v>0.43528728961114338</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D5" si="1">C3</f>
+        <v>0.43528728961114338</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E5" si="2">B3-D3</f>
+        <v>-0.13528728961114339</v>
+      </c>
+      <c r="F3" s="1">
+        <v>500</v>
+      </c>
+      <c r="G3" s="6">
+        <v>60</v>
+      </c>
+      <c r="H3" s="6">
+        <f t="shared" ref="H3:H4" si="3">F3*G3</f>
+        <v>30000</v>
+      </c>
+      <c r="I3" s="8">
+        <f>B3*SUM(H:H)</f>
+        <v>20676</v>
+      </c>
+      <c r="J3" s="9">
+        <f t="shared" ref="J3:J5" si="4">(I3-H3)/G3</f>
+        <v>-155.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="19">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.34677887405687752</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.34677887405687752</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.14677887405687751</v>
+      </c>
+      <c r="F4" s="1">
+        <v>239</v>
+      </c>
+      <c r="G4" s="6">
+        <v>100</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" si="3"/>
+        <v>23900</v>
+      </c>
+      <c r="I4" s="8">
+        <f>B4*SUM(H:H)</f>
+        <v>13784</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" si="4"/>
+        <v>-101.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="19">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>7.8351712130005802E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
+        <v>7.8351712130005802E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1648287869994204E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>100</v>
+      </c>
+      <c r="G5" s="6">
+        <v>54</v>
+      </c>
+      <c r="H5" s="5">
+        <f>F5*G5</f>
+        <v>5400</v>
+      </c>
+      <c r="I5" s="8">
+        <f>B5*SUM(H:H)</f>
+        <v>6892</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="4"/>
+        <v>27.62962962962963</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>